<commit_message>
Schedule Baseline change & study progress
</commit_message>
<xml_diff>
--- a/PMP Study Schedule.xlsx
+++ b/PMP Study Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,40 @@
     <author>Eric Smith</author>
   </authors>
   <commentList>
+    <comment ref="B16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eric Smith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Baseline Changed</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eric Smith</author>
+  </authors>
+  <commentList>
     <comment ref="F4" authorId="0">
       <text>
         <r>
@@ -29,7 +63,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Eric Smith:</t>
         </r>
@@ -38,7 +72,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Started +1</t>
@@ -53,7 +87,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Eric Smith:</t>
         </r>
@@ -62,7 +96,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Started +2</t>
@@ -77,7 +111,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Eric Smith:</t>
         </r>
@@ -86,7 +120,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Started +4</t>
@@ -101,7 +135,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Eric Smith:</t>
         </r>
@@ -110,7 +144,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Started +6</t>
@@ -122,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="40">
   <si>
     <t>June</t>
   </si>
@@ -157,24 +191,6 @@
     <t>7-  Project Cost</t>
   </si>
   <si>
-    <t>8 - Project Quality</t>
-  </si>
-  <si>
-    <t>9 - Human Resources</t>
-  </si>
-  <si>
-    <t>10 - Communication</t>
-  </si>
-  <si>
-    <t>11 - Risk Management</t>
-  </si>
-  <si>
-    <t>12 - Procurement Management</t>
-  </si>
-  <si>
-    <t>13 - Stakeholder Management</t>
-  </si>
-  <si>
     <t>Practice Tests</t>
   </si>
   <si>
@@ -204,12 +220,69 @@
   <si>
     <t>PMP Study Schedule - ACTUAL</t>
   </si>
+  <si>
+    <t>10 - Communication (w/ Crowe)</t>
+  </si>
+  <si>
+    <t>5 - Project Scope (w/ Crowe)</t>
+  </si>
+  <si>
+    <t>6 - Project Time (w/ Crowe)</t>
+  </si>
+  <si>
+    <t>7-  Project Cost (w/ Crowe)</t>
+  </si>
+  <si>
+    <t>8 - Project Quality (w/ Crowe)</t>
+  </si>
+  <si>
+    <t>9 - Human Resources (w/Crowe)</t>
+  </si>
+  <si>
+    <t>11 - Risk Management (w/ Crowe)</t>
+  </si>
+  <si>
+    <t>12 - Procurement (w/ Crowe)</t>
+  </si>
+  <si>
+    <t>13 - Stakeholders (w/ Crowe)</t>
+  </si>
+  <si>
+    <t>TEST!!</t>
+  </si>
+  <si>
+    <t>No study. Idlewild.</t>
+  </si>
+  <si>
+    <t>No Study. Idlewild.</t>
+  </si>
+  <si>
+    <t>Decision: Move Test Date or No?</t>
+  </si>
+  <si>
+    <t>Develop First Pass Network Diagram</t>
+  </si>
+  <si>
+    <t>Read Heldman Book</t>
+  </si>
+  <si>
+    <t>Use InSite Website tools</t>
+  </si>
+  <si>
+    <t>Practice Test in Crowe Book</t>
+  </si>
+  <si>
+    <t>Practice Test - InSite</t>
+  </si>
+  <si>
+    <t>Pratice Test - Heldman?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,17 +332,25 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +360,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -396,6 +489,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -409,6 +511,27 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,21 +834,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="12.7109375" customWidth="1"/>
+    <col min="1" max="15" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -852,9 +975,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="O4" s="13"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -1006,9 +1127,7 @@
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="I8" s="9"/>
       <c r="J8" s="13" t="s">
         <v>5</v>
       </c>
@@ -1024,9 +1143,7 @@
       <c r="N8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="O8" s="13"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -1178,9 +1295,7 @@
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="I12" s="9"/>
       <c r="J12" s="13" t="s">
         <v>5</v>
       </c>
@@ -1196,8 +1311,8 @@
       <c r="N12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="O12" s="13" t="s">
-        <v>5</v>
+      <c r="O12" s="28" t="s">
+        <v>13</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
@@ -1225,7 +1340,7 @@
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="O13" s="29"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
@@ -1252,7 +1367,7 @@
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
+      <c r="O14" s="30"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -1333,28 +1448,28 @@
     </row>
     <row r="16" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>5</v>
+      <c r="B16" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>25</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="1"/>
       <c r="I16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>5</v>
@@ -1368,9 +1483,7 @@
       <c r="N16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="O16" s="13"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
@@ -1384,15 +1497,15 @@
     </row>
     <row r="17" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="14"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="14"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="1"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="14"/>
+      <c r="J17" s="17"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
@@ -1411,15 +1524,15 @@
     </row>
     <row r="18" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="15"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="15"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="1"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="15"/>
+      <c r="J18" s="18"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
@@ -1493,20 +1606,18 @@
     </row>
     <row r="20" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>11</v>
+      <c r="B20" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="I20" s="9"/>
       <c r="J20" s="13" t="s">
         <v>5</v>
       </c>
@@ -1522,9 +1633,7 @@
       <c r="N20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="O20" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="O20" s="13"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
@@ -1538,8 +1647,8 @@
     </row>
     <row r="21" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1565,8 +1674,8 @@
     </row>
     <row r="22" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1630,9 +1739,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="I24" s="9"/>
       <c r="J24" s="13" t="s">
         <v>5</v>
       </c>
@@ -1817,14 +1924,14 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>5</v>
+      <c r="D30" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="1"/>
@@ -1842,9 +1949,7 @@
       <c r="N30" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="O30" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="O30" s="13"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
@@ -1860,9 +1965,9 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="14"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="9"/>
-      <c r="F31" s="14"/>
+      <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="1"/>
       <c r="I31" s="3"/>
@@ -1887,9 +1992,9 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="15"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="15"/>
+      <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="1"/>
       <c r="I32" s="3"/>
@@ -1983,39 +2088,39 @@
         <v>5</v>
       </c>
       <c r="C34" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="M34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="O34" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O34" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
@@ -2151,40 +2256,40 @@
     </row>
     <row r="38" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
-      <c r="B38" s="13" t="s">
-        <v>5</v>
+      <c r="B38" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>15</v>
+      <c r="D38" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="1"/>
       <c r="I38" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K38" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M38" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="N38" s="18" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M38" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="O38" s="9"/>
       <c r="P38" s="4"/>
@@ -2200,19 +2305,19 @@
     </row>
     <row r="39" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
-      <c r="B39" s="14"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="14"/>
       <c r="D39" s="9"/>
       <c r="E39" s="14"/>
-      <c r="F39" s="9"/>
+      <c r="F39" s="25"/>
       <c r="G39" s="9"/>
       <c r="H39" s="1"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="18"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="21"/>
       <c r="O39" s="9"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
@@ -2227,19 +2332,19 @@
     </row>
     <row r="40" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="15"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="15"/>
       <c r="D40" s="10"/>
       <c r="E40" s="15"/>
-      <c r="F40" s="10"/>
+      <c r="F40" s="26"/>
       <c r="G40" s="10"/>
       <c r="H40" s="1"/>
       <c r="I40" s="10"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="19"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="22"/>
       <c r="O40" s="10"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
@@ -2321,11 +2426,11 @@
     </row>
     <row r="42" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
-      <c r="B42" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>16</v>
+      <c r="B42" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>5</v>
@@ -2333,11 +2438,11 @@
       <c r="E42" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F42" s="9" t="s">
-        <v>23</v>
+      <c r="F42" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="9"/>
@@ -2360,11 +2465,11 @@
     </row>
     <row r="43" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
-      <c r="F43" s="9"/>
+      <c r="F43" s="14"/>
       <c r="G43" s="9"/>
       <c r="H43" s="4"/>
       <c r="I43" s="9"/>
@@ -2387,11 +2492,11 @@
     </row>
     <row r="44" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
-      <c r="F44" s="10"/>
+      <c r="F44" s="15"/>
       <c r="G44" s="10"/>
       <c r="H44" s="4"/>
       <c r="I44" s="10"/>
@@ -2469,10 +2574,10 @@
     </row>
     <row r="46" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>5</v>
@@ -3016,6 +3121,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3023,8 +3129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3034,7 +3140,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -3316,7 +3422,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="1"/>
       <c r="I8" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>5</v>
@@ -3488,7 +3594,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="1"/>
       <c r="I12" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J12" s="13" t="s">
         <v>5</v>
@@ -3642,25 +3748,19 @@
     </row>
     <row r="16" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="B16" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="9"/>
       <c r="H16" s="1"/>
       <c r="I16" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>5</v>
@@ -3694,7 +3794,7 @@
     <row r="17" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="14"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -3721,7 +3821,7 @@
     <row r="18" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="15"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -3802,19 +3902,15 @@
     </row>
     <row r="20" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J20" s="13" t="s">
         <v>5</v>
@@ -3940,7 +4036,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J24" s="13" t="s">
         <v>5</v>
@@ -4126,15 +4222,11 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="D30" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="9"/>
       <c r="H30" s="1"/>
       <c r="I30" s="3"/>
@@ -4169,7 +4261,7 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="9"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="9"/>
@@ -4196,7 +4288,7 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="10"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="10"/>
@@ -4288,25 +4380,15 @@
     </row>
     <row r="34" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
-      <c r="B34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="1"/>
       <c r="I34" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J34" s="13" t="s">
         <v>5</v>
@@ -4324,7 +4406,7 @@
         <v>5</v>
       </c>
       <c r="O34" s="13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
@@ -4460,40 +4542,34 @@
     </row>
     <row r="38" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
-      <c r="B38" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="9"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K38" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M38" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="N38" s="18" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M38" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="O38" s="9"/>
       <c r="P38" s="4"/>
@@ -4513,15 +4589,15 @@
       <c r="C39" s="14"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
       <c r="H39" s="1"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="18"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="21"/>
       <c r="O39" s="9"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
@@ -4540,15 +4616,15 @@
       <c r="C40" s="15"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
       <c r="H40" s="1"/>
       <c r="I40" s="10"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="19"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="22"/>
       <c r="O40" s="10"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
@@ -4629,24 +4705,16 @@
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="A42" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
       <c r="G42" s="9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="9"/>
@@ -4668,7 +4736,7 @@
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
@@ -4695,7 +4763,7 @@
       <c r="Y43" s="4"/>
     </row>
     <row r="44" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
@@ -4778,10 +4846,10 @@
     </row>
     <row r="46" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Schedule & Exam Update
</commit_message>
<xml_diff>
--- a/PMP Study Schedule.xlsx
+++ b/PMP Study Schedule.xlsx
@@ -21,6 +21,30 @@
     <author>Eric Smith</author>
   </authors>
   <commentList>
+    <comment ref="E15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eric Smith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Baseline changed.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B16" authorId="0">
       <text>
         <r>
@@ -156,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="40">
   <si>
     <t>June</t>
   </si>
@@ -282,7 +306,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +372,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -474,12 +511,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -488,6 +519,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -510,20 +553,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -532,6 +566,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -847,23 +884,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -876,7 +913,7 @@
       <c r="Y1" s="4"/>
     </row>
     <row r="2" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
@@ -886,7 +923,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="26" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="1"/>
@@ -907,7 +944,7 @@
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -932,7 +969,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="12"/>
+      <c r="I3" s="26"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -954,17 +991,17 @@
     </row>
     <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="14"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="9"/>
@@ -975,7 +1012,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="13"/>
+      <c r="O4" s="11"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -989,11 +1026,11 @@
     </row>
     <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="14"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="9"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1002,7 +1039,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="14"/>
+      <c r="O5" s="12"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -1016,11 +1053,11 @@
     </row>
     <row r="6" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="15"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="10"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1029,7 +1066,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="15"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -1113,13 +1150,13 @@
       <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="C8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -1128,22 +1165,22 @@
       <c r="G8" s="9"/>
       <c r="H8" s="1"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O8" s="13"/>
+      <c r="J8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="11"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -1158,19 +1195,19 @@
     <row r="9" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="1"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -1185,19 +1222,19 @@
     <row r="10" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="1"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -1278,40 +1315,40 @@
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="B12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="1"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O12" s="28" t="s">
+      <c r="J12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" s="27" t="s">
         <v>13</v>
       </c>
       <c r="P12" s="4"/>
@@ -1327,20 +1364,20 @@
     </row>
     <row r="13" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="14"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="9"/>
       <c r="H13" s="1"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="29"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="28"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
@@ -1354,20 +1391,20 @@
     </row>
     <row r="14" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="15"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="10"/>
       <c r="H14" s="1"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="30"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="29"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -1448,19 +1485,19 @@
     </row>
     <row r="16" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="14" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="9"/>
@@ -1468,22 +1505,22 @@
       <c r="I16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="16" t="s">
+      <c r="J16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O16" s="13"/>
+      <c r="K16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16" s="11"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
@@ -1499,18 +1536,18 @@
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="14"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="1"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -1526,18 +1563,18 @@
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="1"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -1606,10 +1643,10 @@
     </row>
     <row r="20" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="1"/>
@@ -1618,22 +1655,22 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O20" s="13"/>
+      <c r="J20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="11"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
@@ -1648,19 +1685,19 @@
     <row r="21" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="14"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
@@ -1675,19 +1712,19 @@
     <row r="22" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="15"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
@@ -1740,7 +1777,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="K24" s="1"/>
@@ -1769,7 +1806,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="14"/>
+      <c r="J25" s="12"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1796,7 +1833,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="15"/>
+      <c r="J26" s="13"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1841,7 +1878,7 @@
       <c r="Y27" s="4"/>
     </row>
     <row r="28" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="1"/>
@@ -1851,10 +1888,10 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="J28" s="12"/>
+      <c r="J28" s="26"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1872,7 +1909,7 @@
       <c r="Y28" s="4"/>
     </row>
     <row r="29" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2">
@@ -1888,8 +1925,8 @@
         <v>4</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
       <c r="K29" s="2">
         <v>1</v>
       </c>
@@ -1924,32 +1961,32 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="14" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="1"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O30" s="13"/>
+      <c r="K30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O30" s="11"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
@@ -1965,18 +2002,18 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="25"/>
+      <c r="D31" s="16"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="1"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
@@ -1992,18 +2029,18 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="26"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="1"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -2084,19 +2121,19 @@
     </row>
     <row r="34" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="23" t="s">
+      <c r="D34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G34" s="9" t="s">
@@ -2104,22 +2141,22 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="9"/>
-      <c r="J34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O34" s="13" t="s">
+      <c r="J34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O34" s="11" t="s">
         <v>13</v>
       </c>
       <c r="P34" s="4"/>
@@ -2135,20 +2172,20 @@
     </row>
     <row r="35" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
-      <c r="B35" s="14"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="14"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="14"/>
+      <c r="F35" s="12"/>
       <c r="G35" s="9"/>
       <c r="H35" s="1"/>
       <c r="I35" s="9"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
@@ -2162,20 +2199,20 @@
     </row>
     <row r="36" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="15"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="15"/>
+      <c r="D36" s="13"/>
       <c r="E36" s="10"/>
-      <c r="F36" s="15"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="10"/>
       <c r="H36" s="1"/>
       <c r="I36" s="10"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
@@ -2256,39 +2293,41 @@
     </row>
     <row r="38" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="23" t="s">
+      <c r="C38" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="24" t="s">
+      <c r="F38" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="9"/>
+      <c r="G38" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J38" s="19" t="s">
+      <c r="J38" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="K38" s="19" t="s">
+      <c r="K38" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="L38" s="19" t="s">
+      <c r="L38" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="M38" s="19" t="s">
+      <c r="M38" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N38" s="21" t="s">
+      <c r="N38" s="23" t="s">
         <v>30</v>
       </c>
       <c r="O38" s="9"/>
@@ -2306,18 +2345,18 @@
     <row r="39" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
-      <c r="C39" s="14"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="9"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="9"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
       <c r="H39" s="1"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="23"/>
       <c r="O39" s="9"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
@@ -2333,18 +2372,18 @@
     <row r="40" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
-      <c r="C40" s="15"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="10"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="10"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
       <c r="H40" s="1"/>
       <c r="I40" s="10"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="24"/>
       <c r="O40" s="10"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
@@ -2425,20 +2464,22 @@
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="23" t="s">
+      <c r="A42" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="13" t="s">
+      <c r="C42" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G42" s="9" t="s">
@@ -2464,12 +2505,12 @@
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="9"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
       <c r="G43" s="9"/>
       <c r="H43" s="4"/>
       <c r="I43" s="9"/>
@@ -2491,12 +2532,12 @@
       <c r="Y43" s="4"/>
     </row>
     <row r="44" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="10"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
       <c r="G44" s="10"/>
       <c r="H44" s="4"/>
       <c r="I44" s="10"/>
@@ -2579,16 +2620,16 @@
       <c r="B46" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F46" s="13" t="s">
+      <c r="C46" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G46" s="7"/>
@@ -2614,10 +2655,10 @@
     <row r="47" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
       <c r="G47" s="7"/>
       <c r="H47" s="4"/>
       <c r="I47" s="9"/>
@@ -2641,10 +2682,10 @@
     <row r="48" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
       <c r="G48" s="7"/>
       <c r="H48" s="4"/>
       <c r="I48" s="10"/>
@@ -2991,40 +3032,75 @@
     </row>
   </sheetData>
   <mergeCells count="127">
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="I28:J29"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="K30:K32"/>
+    <mergeCell ref="L30:L32"/>
+    <mergeCell ref="M30:M32"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="M42:M44"/>
+    <mergeCell ref="N42:N44"/>
+    <mergeCell ref="O42:O44"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="J46:J48"/>
+    <mergeCell ref="K46:K48"/>
+    <mergeCell ref="L46:L48"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="O34:O36"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="J38:J40"/>
+    <mergeCell ref="K38:K40"/>
+    <mergeCell ref="L38:L40"/>
+    <mergeCell ref="M38:M40"/>
+    <mergeCell ref="N38:N40"/>
+    <mergeCell ref="O38:O40"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="M34:M36"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="J42:J44"/>
+    <mergeCell ref="K42:K44"/>
+    <mergeCell ref="L42:L44"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="C34:C36"/>
@@ -3049,75 +3125,40 @@
     <mergeCell ref="N16:N18"/>
     <mergeCell ref="E30:E32"/>
     <mergeCell ref="F30:F32"/>
-    <mergeCell ref="L42:L44"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="M42:M44"/>
-    <mergeCell ref="N42:N44"/>
-    <mergeCell ref="O42:O44"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="J46:J48"/>
-    <mergeCell ref="K46:K48"/>
-    <mergeCell ref="L46:L48"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="O34:O36"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="J38:J40"/>
-    <mergeCell ref="K38:K40"/>
-    <mergeCell ref="L38:L40"/>
-    <mergeCell ref="M38:M40"/>
-    <mergeCell ref="N38:N40"/>
-    <mergeCell ref="O38:O40"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="M34:M36"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="J42:J44"/>
-    <mergeCell ref="K42:K44"/>
-    <mergeCell ref="G30:G32"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="I28:J29"/>
-    <mergeCell ref="O4:O6"/>
-    <mergeCell ref="K30:K32"/>
-    <mergeCell ref="L30:L32"/>
-    <mergeCell ref="M30:M32"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3139,23 +3180,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -3168,7 +3209,7 @@
       <c r="Y1" s="4"/>
     </row>
     <row r="2" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
@@ -3178,7 +3219,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="26" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="1"/>
@@ -3199,7 +3240,7 @@
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -3224,7 +3265,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="12"/>
+      <c r="I3" s="26"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -3246,14 +3287,14 @@
     </row>
     <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="14"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -3267,7 +3308,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="P4" s="4"/>
@@ -3283,10 +3324,10 @@
     </row>
     <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="14"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="14"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="1"/>
@@ -3296,7 +3337,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="14"/>
+      <c r="O5" s="12"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -3310,10 +3351,10 @@
     </row>
     <row r="6" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="15"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="15"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="1"/>
@@ -3323,7 +3364,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="15"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -3404,16 +3445,16 @@
     </row>
     <row r="8" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
-      <c r="B8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -3424,22 +3465,22 @@
       <c r="I8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O8" s="13" t="s">
+      <c r="J8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="P8" s="4"/>
@@ -3455,20 +3496,20 @@
     </row>
     <row r="9" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="1"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -3482,20 +3523,20 @@
     </row>
     <row r="10" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="1"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -3576,19 +3617,19 @@
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="9"/>
@@ -3596,22 +3637,22 @@
       <c r="I12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O12" s="13" t="s">
+      <c r="J12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="P12" s="4"/>
@@ -3627,20 +3668,20 @@
     </row>
     <row r="13" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="9"/>
       <c r="H13" s="1"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
@@ -3654,20 +3695,20 @@
     </row>
     <row r="14" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="10"/>
       <c r="H14" s="1"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -3748,36 +3789,36 @@
     </row>
     <row r="16" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="9"/>
       <c r="H16" s="1"/>
       <c r="I16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O16" s="13" t="s">
+      <c r="J16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16" s="11" t="s">
         <v>5</v>
       </c>
       <c r="P16" s="4"/>
@@ -3796,17 +3837,17 @@
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="9"/>
       <c r="H17" s="1"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -3823,17 +3864,17 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="10"/>
       <c r="H18" s="1"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -3903,7 +3944,7 @@
     <row r="20" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="13"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -3912,22 +3953,22 @@
       <c r="I20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O20" s="13" t="s">
+      <c r="J20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="11" t="s">
         <v>5</v>
       </c>
       <c r="P20" s="4"/>
@@ -3944,19 +3985,19 @@
     <row r="21" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="14"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
@@ -3971,19 +4012,19 @@
     <row r="22" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="15"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
@@ -4038,7 +4079,7 @@
       <c r="I24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="K24" s="1"/>
@@ -4067,7 +4108,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="14"/>
+      <c r="J25" s="12"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -4094,7 +4135,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="15"/>
+      <c r="J26" s="13"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -4139,7 +4180,7 @@
       <c r="Y27" s="4"/>
     </row>
     <row r="28" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="1"/>
@@ -4149,10 +4190,10 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="J28" s="12"/>
+      <c r="J28" s="26"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -4170,7 +4211,7 @@
       <c r="Y28" s="4"/>
     </row>
     <row r="29" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2">
@@ -4186,8 +4227,8 @@
         <v>4</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
       <c r="K29" s="2">
         <v>1</v>
       </c>
@@ -4222,28 +4263,28 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
       <c r="G30" s="9"/>
       <c r="H30" s="1"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O30" s="13" t="s">
+      <c r="K30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O30" s="11" t="s">
         <v>5</v>
       </c>
       <c r="P30" s="4"/>
@@ -4261,18 +4302,18 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
       <c r="G31" s="9"/>
       <c r="H31" s="1"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
@@ -4288,18 +4329,18 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
       <c r="G32" s="10"/>
       <c r="H32" s="1"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -4380,32 +4421,32 @@
     </row>
     <row r="34" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
-      <c r="B34" s="13"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="1"/>
       <c r="I34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N34" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="O34" s="13" t="s">
+      <c r="J34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O34" s="11" t="s">
         <v>13</v>
       </c>
       <c r="P34" s="4"/>
@@ -4421,20 +4462,20 @@
     </row>
     <row r="35" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
-      <c r="B35" s="14"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="1"/>
       <c r="I35" s="9"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
@@ -4448,20 +4489,20 @@
     </row>
     <row r="36" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="15"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="1"/>
       <c r="I36" s="10"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
@@ -4542,33 +4583,33 @@
     </row>
     <row r="38" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="24" t="s">
+      <c r="F38" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="G38" s="15" t="s">
         <v>18</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J38" s="19" t="s">
+      <c r="J38" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="K38" s="19" t="s">
+      <c r="K38" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="L38" s="19" t="s">
+      <c r="L38" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="M38" s="19" t="s">
+      <c r="M38" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N38" s="21" t="s">
+      <c r="N38" s="23" t="s">
         <v>16</v>
       </c>
       <c r="O38" s="9"/>
@@ -4585,19 +4626,19 @@
     </row>
     <row r="39" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
       <c r="H39" s="1"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="23"/>
       <c r="O39" s="9"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
@@ -4612,19 +4653,19 @@
     </row>
     <row r="40" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
       <c r="H40" s="1"/>
       <c r="I40" s="10"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="24"/>
       <c r="O40" s="10"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
@@ -4705,7 +4746,7 @@
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B42" s="9"/>
@@ -4736,7 +4777,7 @@
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
@@ -4763,7 +4804,7 @@
       <c r="Y43" s="4"/>
     </row>
     <row r="44" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
@@ -4851,16 +4892,16 @@
       <c r="B46" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F46" s="13" t="s">
+      <c r="C46" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G46" s="7"/>
@@ -4886,10 +4927,10 @@
     <row r="47" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
       <c r="G47" s="7"/>
       <c r="H47" s="4"/>
       <c r="I47" s="9"/>
@@ -4913,10 +4954,10 @@
     <row r="48" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
       <c r="G48" s="7"/>
       <c r="H48" s="4"/>
       <c r="I48" s="10"/>
@@ -5263,67 +5304,48 @@
     </row>
   </sheetData>
   <mergeCells count="127">
-    <mergeCell ref="J46:J48"/>
-    <mergeCell ref="K46:K48"/>
-    <mergeCell ref="L46:L48"/>
-    <mergeCell ref="M42:M44"/>
-    <mergeCell ref="N42:N44"/>
-    <mergeCell ref="O42:O44"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="J42:J44"/>
-    <mergeCell ref="K42:K44"/>
-    <mergeCell ref="L42:L44"/>
-    <mergeCell ref="K38:K40"/>
-    <mergeCell ref="L38:L40"/>
-    <mergeCell ref="M38:M40"/>
-    <mergeCell ref="N38:N40"/>
-    <mergeCell ref="O38:O40"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="J38:J40"/>
-    <mergeCell ref="M30:M32"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="G30:G32"/>
-    <mergeCell ref="K30:K32"/>
-    <mergeCell ref="L30:L32"/>
-    <mergeCell ref="O34:O36"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="M34:M36"/>
-    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
     <mergeCell ref="N20:N22"/>
     <mergeCell ref="O20:O22"/>
     <mergeCell ref="I24:I26"/>
@@ -5348,48 +5370,67 @@
     <mergeCell ref="M16:M18"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="M30:M32"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="K30:K32"/>
+    <mergeCell ref="L30:L32"/>
+    <mergeCell ref="O34:O36"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="M34:M36"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="K38:K40"/>
+    <mergeCell ref="L38:L40"/>
+    <mergeCell ref="M38:M40"/>
+    <mergeCell ref="N38:N40"/>
+    <mergeCell ref="O38:O40"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="J38:J40"/>
+    <mergeCell ref="J46:J48"/>
+    <mergeCell ref="K46:K48"/>
+    <mergeCell ref="L46:L48"/>
+    <mergeCell ref="M42:M44"/>
+    <mergeCell ref="N42:N44"/>
+    <mergeCell ref="O42:O44"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="J42:J44"/>
+    <mergeCell ref="K42:K44"/>
+    <mergeCell ref="L42:L44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>